<commit_message>
Roundup of code and stuff
Everything has run. The code has been added to a rar file that can be
send, including the results. SUCCES!
</commit_message>
<xml_diff>
--- a/Ass2/results/resultsU.xlsx
+++ b/Ass2/results/resultsU.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>bestid</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Ttest answer?</t>
+  </si>
+  <si>
+    <t>Cmp MLS to GLS</t>
+  </si>
+  <si>
+    <t>ILS TO GLS 50</t>
+  </si>
+  <si>
+    <t>ILS TO GLS100</t>
   </si>
 </sst>
 </file>
@@ -104,11 +113,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,13 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,38 +211,29 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>85935</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>211982</c:v>
+                  <c:v>1606</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>456</c:v>
+                  <c:v>3621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>700</c:v>
+                  <c:v>6750</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1606</c:v>
+                  <c:v>14729</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3621</c:v>
+                  <c:v>21387</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6750</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14729</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>21387</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>310431</c:v>
                 </c:pt>
               </c:numCache>
@@ -232,61 +241,52 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:f>Sheet1!$I$4:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>17069</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45307</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>187</c:v>
+                  <c:v>1492</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>295</c:v>
+                  <c:v>2544</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>701</c:v>
+                  <c:v>4950</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1492</c:v>
+                  <c:v>6933</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2544</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4950</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6933</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>28861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="141968128"/>
-        <c:axId val="141962240"/>
+        <c:axId val="62386560"/>
+        <c:axId val="62437632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141968128"/>
+        <c:axId val="62386560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141962240"/>
+        <c:crossAx val="62437632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141962240"/>
+        <c:axId val="62437632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -294,7 +294,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141968128"/>
+        <c:crossAx val="62386560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -307,7 +307,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -325,7 +325,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -634,10 +634,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,9 +645,8 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -655,10 +654,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="3"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -697,13 +696,13 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>6.4</v>
       </c>
       <c r="F2">
         <v>6.5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>4.3066666666666604</v>
       </c>
       <c r="H2">
@@ -726,16 +725,16 @@
       <c r="C3">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>5.2666666666666604</v>
       </c>
       <c r="F3">
         <v>6</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>3.1955555555555502</v>
       </c>
       <c r="H3">
@@ -756,25 +755,25 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2">
-        <v>47.6666666666666</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42.033333333333303</v>
       </c>
       <c r="F4">
-        <v>48</v>
-      </c>
-      <c r="G4" s="3">
-        <v>64.755555555555503</v>
+        <v>45</v>
+      </c>
+      <c r="G4" s="2">
+        <v>89.432222222222194</v>
       </c>
       <c r="H4">
-        <v>456</v>
+        <v>700</v>
       </c>
       <c r="I4">
-        <v>187</v>
+        <v>295</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -788,25 +787,25 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2">
-        <v>42.033333333333303</v>
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40.033333333333303</v>
       </c>
       <c r="F5">
-        <v>45</v>
-      </c>
-      <c r="G5" s="3">
-        <v>89.432222222222194</v>
+        <v>37.5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>118.765555555555</v>
       </c>
       <c r="H5">
-        <v>700</v>
+        <v>1606</v>
       </c>
       <c r="I5">
-        <v>295</v>
+        <v>701</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -820,25 +819,25 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2">
-        <v>40.033333333333303</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
+        <v>38.1</v>
       </c>
       <c r="F6">
-        <v>37.5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>118.765555555555</v>
+        <v>36.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>81.489999999999995</v>
       </c>
       <c r="H6">
-        <v>1606</v>
+        <v>3621</v>
       </c>
       <c r="I6">
-        <v>701</v>
+        <v>1492</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -852,25 +851,25 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>24</v>
       </c>
-      <c r="E7" s="2">
-        <v>38.1</v>
+      <c r="E7" s="1">
+        <v>37.866666666666603</v>
       </c>
       <c r="F7">
-        <v>36.5</v>
-      </c>
-      <c r="G7" s="3">
-        <v>81.489999999999995</v>
+        <v>37.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>51.115555555555503</v>
       </c>
       <c r="H7">
-        <v>3621</v>
+        <v>6750</v>
       </c>
       <c r="I7">
-        <v>1492</v>
+        <v>2544</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -884,25 +883,25 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2">
-        <v>37.866666666666603</v>
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>33.866666666666603</v>
       </c>
       <c r="F8">
-        <v>37.5</v>
-      </c>
-      <c r="G8" s="3">
-        <v>51.115555555555503</v>
+        <v>34</v>
+      </c>
+      <c r="G8" s="2">
+        <v>81.115555555555503</v>
       </c>
       <c r="H8">
-        <v>6750</v>
+        <v>14729</v>
       </c>
       <c r="I8">
-        <v>2544</v>
+        <v>4950</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -916,25 +915,25 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2">
-        <v>33.866666666666603</v>
+        <v>23</v>
+      </c>
+      <c r="E9" s="1">
+        <v>35.566666666666599</v>
       </c>
       <c r="F9">
-        <v>34</v>
-      </c>
-      <c r="G9" s="3">
-        <v>81.115555555555503</v>
+        <v>35.5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>50.112222222222201</v>
       </c>
       <c r="H9">
-        <v>14729</v>
+        <v>21387</v>
       </c>
       <c r="I9">
-        <v>4950</v>
+        <v>6933</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -942,31 +941,31 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2">
-        <v>35.566666666666599</v>
+        <v>18</v>
+      </c>
+      <c r="E10" s="1">
+        <v>24.433333333333302</v>
       </c>
       <c r="F10">
-        <v>35.5</v>
-      </c>
-      <c r="G10" s="3">
-        <v>50.112222222222201</v>
+        <v>24.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>10.845555555555499</v>
       </c>
       <c r="H10">
-        <v>21387</v>
+        <v>310431</v>
       </c>
       <c r="I10">
-        <v>6933</v>
+        <v>28861</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -974,59 +973,47 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2">
-        <v>24.433333333333302</v>
-      </c>
-      <c r="F11">
-        <v>24.5</v>
-      </c>
-      <c r="G11" s="3">
-        <v>10.845555555555499</v>
-      </c>
-      <c r="H11">
-        <v>310431</v>
-      </c>
-      <c r="I11">
-        <v>28861</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="E13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" ref="D15:D20" si="0">ABS($E$10-E4)</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <f>($G$10+G4)/30</f>
+        <v>3.3425925925925895</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" ref="F15:F20" si="1">D15/SQRT(E15)</f>
+        <v>9.6265560673301867</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1034,19 +1021,19 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16">
-        <f>ABS($E$11-E4)</f>
-        <v>23.233333333333299</v>
-      </c>
-      <c r="E16">
-        <f>($G$11+G4)/30</f>
-        <v>2.5200370370370337</v>
-      </c>
-      <c r="F16">
-        <f>D16/SQRT(E16)</f>
-        <v>14.635516765534899</v>
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E20" si="2">($G$10+G5)/30</f>
+        <v>4.32037037037035</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>7.5052317800325499</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1054,19 +1041,19 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D22" si="0">ABS($E$11-E5)</f>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="E17">
-        <f>($G$11+G5)/30</f>
-        <v>3.3425925925925895</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ref="F17:F22" si="1">D17/SQRT(E17)</f>
-        <v>9.6265560673301867</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>13.6666666666667</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0778518518518494</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>7.7900231104361968</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1074,19 +1061,19 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>15.600000000000001</v>
-      </c>
-      <c r="E18">
-        <f t="shared" ref="E17:E22" si="2">($G$11+G6)/30</f>
-        <v>4.32037037037035</v>
-      </c>
-      <c r="F18">
+        <v>13.433333333333302</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0653703703703665</v>
+      </c>
+      <c r="F18" s="1">
         <f t="shared" si="1"/>
-        <v>7.5052317800325499</v>
+        <v>9.3472707011062557</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1094,19 +1081,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>13.6666666666667</v>
-      </c>
-      <c r="E19">
+        <v>9.4333333333333016</v>
+      </c>
+      <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>3.0778518518518494</v>
-      </c>
-      <c r="F19">
+        <v>3.0653703703703665</v>
+      </c>
+      <c r="F19" s="1">
         <f t="shared" si="1"/>
-        <v>7.7900231104361968</v>
+        <v>5.3879518157574404</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1114,59 +1101,346 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>13.433333333333302</v>
-      </c>
-      <c r="E20">
+        <v>11.133333333333297</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>2.0653703703703665</v>
-      </c>
-      <c r="F20">
+        <v>2.0319259259259232</v>
+      </c>
+      <c r="F20" s="1">
         <f t="shared" si="1"/>
-        <v>9.3472707011062557</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>9.4333333333333016</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>3.0653703703703665</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>5.3879518157574404</v>
+        <v>7.8103640312197369</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1">
+        <f>ABS($E$10-E2)</f>
+        <v>18.033333333333303</v>
+      </c>
+      <c r="E23" s="1">
+        <f>($G$10+G2)/30</f>
+        <v>0.50507407407407201</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:F28" si="3">D23/SQRT(E23)</f>
+        <v>25.374557194550913</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <f>ABS($E$10-E3)</f>
+        <v>19.166666666666643</v>
+      </c>
+      <c r="E24" s="1">
+        <f>($G$10+G3)/30</f>
+        <v>0.46803703703703498</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="3"/>
+        <v>28.01602261468101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="1">
+        <f>ABS($E$2-E4)</f>
+        <v>35.633333333333304</v>
+      </c>
+      <c r="E27" s="1">
+        <f>($G$2+G4)/30</f>
+        <v>3.1246296296296285</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" ref="F27:F32" si="4">D27/SQRT(E27)</f>
+        <v>20.158451919349968</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" ref="D28:D32" si="5">ABS($E$2-E5)</f>
+        <v>33.633333333333304</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" ref="E28:E32" si="6">($G$2+G5)/30</f>
+        <v>4.1024074074073882</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="4"/>
+        <v>16.605444968446346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="5"/>
+        <v>31.700000000000003</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="6"/>
+        <v>2.8598888888888885</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="4"/>
+        <v>18.744967077740128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="5"/>
+        <v>31.466666666666605</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="6"/>
+        <v>1.8474074074074054</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="4"/>
+        <v>23.150981037857445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="5"/>
+        <v>27.466666666666605</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="6"/>
+        <v>2.8474074074074052</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="4"/>
+        <v>16.27725441978496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>11.133333333333297</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>2.0319259259259232</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>7.8103640312197369</v>
+      <c r="D32" s="1">
+        <f t="shared" si="5"/>
+        <v>29.1666666666666</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="6"/>
+        <v>1.8139629629629619</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="4"/>
+        <v>21.655718155627682</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="1">
+        <f>ABS($E$2-E4)</f>
+        <v>35.633333333333304</v>
+      </c>
+      <c r="E35" s="1">
+        <f>($G$2+G4)/30</f>
+        <v>3.1246296296296285</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" ref="F35:F40" si="7">D35/SQRT(E35)</f>
+        <v>20.158451919349968</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" ref="D36:D40" si="8">ABS($E$2-E5)</f>
+        <v>33.633333333333304</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:E40" si="9">($G$2+G5)/30</f>
+        <v>4.1024074074073882</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="7"/>
+        <v>16.605444968446346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="8"/>
+        <v>31.700000000000003</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="9"/>
+        <v>2.8598888888888885</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="7"/>
+        <v>18.744967077740128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="8"/>
+        <v>31.466666666666605</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="9"/>
+        <v>1.8474074074074054</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="7"/>
+        <v>23.150981037857445</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="8"/>
+        <v>27.466666666666605</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="9"/>
+        <v>2.8474074074074052</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="7"/>
+        <v>16.27725441978496</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="8"/>
+        <v>29.1666666666666</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="9"/>
+        <v>1.8139629629629619</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="7"/>
+        <v>21.655718155627682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>